<commit_message>
change logname plus if
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4584" yWindow="2880" windowWidth="17280" windowHeight="8964" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4068" yWindow="3396" windowWidth="17280" windowHeight="8964" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -444,10 +444,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A11" sqref="A1:C211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="17.4"/>
@@ -455,15 +455,20 @@
     <row r="1">
       <c r="A1" s="0" t="inlineStr">
         <is>
+          <t>202011181595host1</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:09:05.648934</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B1" s="0" t="inlineStr">
-        <is>
-          <t>2020-11-18 13:50:33.215895</t>
-        </is>
-      </c>
-      <c r="C1" s="0" t="inlineStr">
+      <c r="D1" s="0" t="inlineStr">
         <is>
           <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
         </is>
@@ -472,15 +477,20 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
+          <t>202011181595host1</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:09:05.739690</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>2020-11-18 13:50:33.249664</t>
-        </is>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
+      <c r="D2" s="0" t="inlineStr">
         <is>
           <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
         </is>
@@ -489,15 +499,20 @@
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
+          <t>202011181596host2</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:09:06.130290</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>2020-11-18 13:50:34.415742</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
+      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
         </is>
@@ -506,15 +521,20 @@
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
+          <t>202011181597host1</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:09:07.058974</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
-      <c r="B4" s="0" t="inlineStr">
-        <is>
-          <t>2020-11-18 13:50:34.982280</t>
-        </is>
-      </c>
-      <c r="C4" s="0" t="inlineStr">
+      <c r="D4" s="0" t="inlineStr">
         <is>
           <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
         </is>
@@ -523,15 +543,20 @@
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
+          <t>202011181598host1</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:09:08.108657</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
-      <c r="B5" s="0" t="inlineStr">
-        <is>
-          <t>2020-11-18 13:50:35.245280</t>
-        </is>
-      </c>
-      <c r="C5" s="0" t="inlineStr">
+      <c r="D5" s="0" t="inlineStr">
         <is>
           <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
         </is>
@@ -540,15 +565,20 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>202011181598host1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:09:08.633293</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2020-11-18 13:50:35.418429</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
         </is>
@@ -557,15 +587,20 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>202011181599host2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:09:09.236645</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>7</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2020-11-18 13:50:35.569774</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
         </is>
@@ -574,15 +609,20 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>202011181599host1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:09:09.775286</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>8</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2020-11-18 13:50:35.731862</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
         </is>
@@ -591,15 +631,20 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>2020111815910host2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:09:10.072783</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>9</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2020-11-18 13:52:01.422989</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
         </is>
@@ -608,15 +653,20 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>2020111815910host1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:09:10.210922</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>10</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2020-11-18 13:52:01.508244</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
         </is>
@@ -625,15 +675,20 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>2020111815910host2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:09:10.466494</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>11</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2020-11-18 13:52:01.674837</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
         </is>
@@ -642,15 +697,20 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>2020111815910host3</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:09:10.600160</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>12</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2020-11-18 13:52:02.224277</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
         </is>
@@ -660,15 +720,20 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>2020111815910host4</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:09:10.755138</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>13</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2020-11-18 13:52:02.476241</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
         </is>
@@ -677,15 +742,86 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>2020111815911host5</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:09:11.019939</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>14</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>2020-11-18 13:52:02.709984</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2020111815911host1</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:09:11.172573</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2020111815911host2</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:09:11.319184</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2020111815911host3</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:09:11.448834</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
         <is>
           <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
         </is>

</xml_diff>

<commit_message>
plus second per people
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,53 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leeseungkyu\PycharmProjects\localhostwebserver\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25F95E1-10F8-4208-89D6-EA9449BC921E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4476" yWindow="996" windowWidth="17280" windowHeight="8964" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
+      <name val="맑은 고딕"/>
+      <charset val="129"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="맑은 고딕"/>
+      <charset val="129"/>
+      <family val="2"/>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -63,31 +53,93 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -387,21 +439,588 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" workbookViewId="0">
-      <selection activeCell="K206" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="17.4"/>
   <sheetData>
-    <row r="12" spans="5:5" x14ac:dyDescent="0.4">
-      <c r="E12" s="1"/>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>2020111816154host0</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 16:01:54.369793</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E1" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>2020111816154host1</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 16:01:54.403701</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E2" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>2020111816155host0</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 16:01:55.165889</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E3" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>2020111816156host0</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 16:01:56.207521</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>2020111816156host1</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 16:01:56.971260</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E5" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>2020111816157host0</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 16:01:57.145530</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>2020111816157host1</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 16:01:57.278273</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>2020111816157host2</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 16:01:57.715043</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E8" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>2020111816158host0</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 16:01:58.241076</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E9" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>2020111816158host1</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 16:01:58.431732</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E10" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>2020111816158host2</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 16:01:58.736322</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E11" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>2020111816158host3</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 16:01:58.838090</t>
+        </is>
+      </c>
+      <c r="C12" s="0" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>2020111816159host0</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 16:01:59.513694</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E13" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="inlineStr">
+        <is>
+          <t>2020111816159host1</t>
+        </is>
+      </c>
+      <c r="B14" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 16:01:59.705053</t>
+        </is>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E14" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t>2020111815586host1</t>
+        </is>
+      </c>
+      <c r="B15" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:58:06.696088</t>
+        </is>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E15" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="inlineStr">
+        <is>
+          <t>2020111815588host0</t>
+        </is>
+      </c>
+      <c r="B16" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:58:08.300073</t>
+        </is>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E16" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="inlineStr">
+        <is>
+          <t>20201118155810host0</t>
+        </is>
+      </c>
+      <c r="B17" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:58:10.315484</t>
+        </is>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E17" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>20201118155812host0</t>
+        </is>
+      </c>
+      <c r="B18" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:58:12.053975</t>
+        </is>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E18" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="inlineStr">
+        <is>
+          <t>20201118155813host0</t>
+        </is>
+      </c>
+      <c r="B19" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:58:13.545390</t>
+        </is>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E19" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="inlineStr">
+        <is>
+          <t>20201118155814host0</t>
+        </is>
+      </c>
+      <c r="B20" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:58:14.258891</t>
+        </is>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E20" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="inlineStr">
+        <is>
+          <t>20201118155814host1</t>
+        </is>
+      </c>
+      <c r="B21" s="0" t="inlineStr">
+        <is>
+          <t>2020-11-18 15:58:14.813893</t>
+        </is>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E21" s="0" t="inlineStr">
+        <is>
+          <t>b'GET /testserver.html HTTP/1.1\r\nHost: localhost:8000\r\nConnection: keep-alive\r\nCache-Control: max-age=0\r\nUpgrade-Insecure-Requests: 1\r\nUser-Agent: Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/86.0.4240.198 Safari/537.36\r\nAccept: text/html,application/xhtml+xml,application/xml;q=0.9,image/avif,image/webp,image/apng,*/*;q=0.8,application/signed-exchange;v=b3;q=0.9\r\nSec-Fetch-Site: none\r\nSec-Fetch-Mode: navigate\r\nSec-Fetch-User: ?1\r\nSec-Fetch-Dest: document\r\nAccept-Encoding: gzip, deflate, br\r\nAccept-Language: ko-KR,ko;q=0.9,en-US;q=0.8,en;q=0.7,ja;q=0.6\r\n\r\n'</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" paperSize="9" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>